<commit_message>
updated control signal names
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">1 (using immediate value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">0 (not reading from memory)</t>
@@ -214,19 +217,19 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M10" activeCellId="0" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.84"/>
@@ -235,7 +238,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="10.83"/>
   </cols>
@@ -316,32 +319,35 @@
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished the opcode and Function codes
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alek\cpre_381\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AB804A-5DD4-444F-8773-D61AAA9BBB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8653BFF2-EE33-4B7B-9B1A-7DA40B6E32C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38805" yWindow="-16515" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,13 +318,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,494 +663,494 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.8125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.3125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.9375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.9375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.1875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.8125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="25.25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="27.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.0625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.5" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.0625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="21.9375" style="3" customWidth="1"/>
-    <col min="16" max="1024" width="10.8125" style="3"/>
+    <col min="1" max="1" width="9.8125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.9375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.9375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.8125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.0625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.0625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.9375" style="1" customWidth="1"/>
+    <col min="16" max="1024" width="10.8125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ALU control now has 6 bits, one additional bit for msb, will allow for slt to work, updated the control and alu object
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alek\cpre_381\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C7BE67-266C-415A-BD9D-174673E6F154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE260EB-DA66-4710-9AEB-037CF9DA8129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -321,10 +321,10 @@
     <t>"000111"</t>
   </si>
   <si>
-    <t>ALUControl (i_ALU_C) [5]</t>
-  </si>
-  <si>
     <t>o_STD_Shift[1]</t>
+  </si>
+  <si>
+    <t>ALUControl (i_ALU_C) [6]</t>
   </si>
 </sst>
 </file>
@@ -829,11 +829,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AML39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -898,13 +898,13 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
@@ -961,8 +961,8 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="str" cm="1">
-        <f t="array" ref="H3">_xlfn.SWITCH(B3, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1020,8 +1020,8 @@
         <v>23</v>
       </c>
       <c r="H4" s="1" t="str" cm="1">
-        <f t="array" ref="H4">_xlfn.SWITCH(B4, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>24</v>
@@ -1079,8 +1079,8 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="str" cm="1">
-        <f t="array" ref="H5">_xlfn.SWITCH(B5, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>00000</v>
+        <f t="array" ref="H5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>000000</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -1138,8 +1138,8 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="str" cm="1">
-        <f t="array" ref="H6">_xlfn.SWITCH(B6, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>00000</v>
+        <f t="array" ref="H6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>000000</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -1198,8 +1198,8 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="str" cm="1">
-        <f t="array" ref="H7">_xlfn.SWITCH(B7, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10011</v>
+        <f t="array" ref="H7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010011</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1258,8 +1258,8 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="str" cm="1">
-        <f t="array" ref="H8">_xlfn.SWITCH(B8, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10011</v>
+        <f t="array" ref="H8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010011</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -1318,8 +1318,8 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="str" cm="1">
-        <f t="array" ref="H9">_xlfn.SWITCH(B9, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10111</v>
+        <f t="array" ref="H9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010111</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -1378,8 +1378,8 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="str" cm="1">
-        <f t="array" ref="H10">_xlfn.SWITCH(B10, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
@@ -1438,8 +1438,8 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="str" cm="1">
-        <f t="array" ref="H11">_xlfn.SWITCH(B11, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10110</v>
+        <f t="array" ref="H11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010110</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -1497,8 +1497,8 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="str" cm="1">
-        <f t="array" ref="H12">_xlfn.SWITCH(B12, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10101</v>
+        <f t="array" ref="H12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010101</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
@@ -1556,8 +1556,8 @@
         <v>1</v>
       </c>
       <c r="H13" s="1" t="str" cm="1">
-        <f t="array" ref="H13">_xlfn.SWITCH(B13, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10101</v>
+        <f t="array" ref="H13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010101</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -1615,8 +1615,8 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="str" cm="1">
-        <f t="array" ref="H14">_xlfn.SWITCH(B14, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10100</v>
+        <f t="array" ref="H14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010100</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -1674,8 +1674,8 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="str" cm="1">
-        <f t="array" ref="H15">_xlfn.SWITCH(B15, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10100</v>
+        <f t="array" ref="H15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010100</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -1733,8 +1733,8 @@
         <v>0</v>
       </c>
       <c r="H16" s="1" t="str" cm="1">
-        <f t="array" ref="H16">_xlfn.SWITCH(B16, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11000</v>
+        <f t="array" ref="H16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="I16" s="7">
         <v>0</v>
@@ -2799,8 +2799,8 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="str" cm="1">
-        <f t="array" ref="H17">_xlfn.SWITCH(B17, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11000</v>
+        <f t="array" ref="H17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -2858,8 +2858,8 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="str" cm="1">
-        <f t="array" ref="H18">_xlfn.SWITCH(B18, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10010</v>
+        <f t="array" ref="H18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010010</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -2917,8 +2917,8 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="str" cm="1">
-        <f t="array" ref="H19">_xlfn.SWITCH(B19, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10001</v>
+        <f t="array" ref="H19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010001</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -2976,8 +2976,8 @@
         <v>0</v>
       </c>
       <c r="H20" s="1" t="str" cm="1">
-        <f t="array" ref="H20">_xlfn.SWITCH(B20, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11001</v>
+        <f t="array" ref="H20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011001</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -3035,8 +3035,8 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="str" cm="1">
-        <f t="array" ref="H21">_xlfn.SWITCH(B21, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -3094,8 +3094,8 @@
         <v>0</v>
       </c>
       <c r="H22" s="1" t="str" cm="1">
-        <f t="array" ref="H22">_xlfn.SWITCH(B22, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11000</v>
+        <f t="array" ref="H22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -3153,8 +3153,8 @@
         <v>0</v>
       </c>
       <c r="H23" s="1" t="str" cm="1">
-        <f t="array" ref="H23">_xlfn.SWITCH(B23, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>01000</v>
+        <f t="array" ref="H23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>001000</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -3212,8 +3212,8 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="str" cm="1">
-        <f t="array" ref="H24">_xlfn.SWITCH(B24, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11000</v>
+        <f t="array" ref="H24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -3271,8 +3271,8 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="str" cm="1">
-        <f t="array" ref="H25">_xlfn.SWITCH(B25, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11000</v>
+        <f t="array" ref="H25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -3330,8 +3330,8 @@
         <v>1</v>
       </c>
       <c r="H26" s="1" t="str" cm="1">
-        <f t="array" ref="H26">_xlfn.SWITCH(B26, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -3388,8 +3388,8 @@
         <v>1</v>
       </c>
       <c r="H27" s="1" t="str" cm="1">
-        <f t="array" ref="H27">_xlfn.SWITCH(B27, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -3446,8 +3446,8 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="str" cm="1">
-        <f t="array" ref="H28">_xlfn.SWITCH(B28, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
@@ -3505,8 +3505,8 @@
         <v>1</v>
       </c>
       <c r="H29" s="1" t="str" cm="1">
-        <f t="array" ref="H29">_xlfn.SWITCH(B29, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I29" s="6">
         <v>1</v>
@@ -4571,8 +4571,8 @@
         <v>1</v>
       </c>
       <c r="H30" s="1" t="str" cm="1">
-        <f t="array" ref="H30">_xlfn.SWITCH(B30, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I30" s="6">
         <v>1</v>
@@ -5637,8 +5637,8 @@
         <v>1</v>
       </c>
       <c r="H31" s="1" t="str" cm="1">
-        <f t="array" ref="H31">_xlfn.SWITCH(B31, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I31" s="6">
         <v>1</v>
@@ -6703,8 +6703,8 @@
         <v>1</v>
       </c>
       <c r="H32" s="1" t="str" cm="1">
-        <f t="array" ref="H32">_xlfn.SWITCH(B32, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10000</v>
+        <f t="array" ref="H32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="I32" s="6">
         <v>1</v>
@@ -7769,8 +7769,8 @@
         <v>0</v>
       </c>
       <c r="H33" s="1" t="str" cm="1">
-        <f t="array" ref="H33">_xlfn.SWITCH(B33, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10010</v>
+        <f t="array" ref="H33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010010</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -7828,8 +7828,8 @@
         <v>0</v>
       </c>
       <c r="H34" s="1" t="str" cm="1">
-        <f t="array" ref="H34">_xlfn.SWITCH(B34, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>10001</v>
+        <f t="array" ref="H34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>010001</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -7887,8 +7887,8 @@
         <v>0</v>
       </c>
       <c r="H35" s="1" t="str" cm="1">
-        <f t="array" ref="H35">_xlfn.SWITCH(B35, "addu", "00000","add", "10000", "subu", "01000","sub", "11000", "srl", "10001", "sra", "11001", "sll", "10010", "and", "10011", "or", "10100", "xor", "10101", "nor", "10110", "lui", "10111", "TODO")</f>
-        <v>11001</v>
+        <f t="array" ref="H35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>011001</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
updated slti in control logic
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alek\cpre_381\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE260EB-DA66-4710-9AEB-037CF9DA8129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA93C5F7-6F75-4F8F-AB5C-148D6EDEE82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -833,7 +833,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="str" cm="1">
-        <f t="array" ref="H3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
       <c r="I3" s="1">
@@ -1020,7 +1020,7 @@
         <v>23</v>
       </c>
       <c r="H4" s="1" t="str" cm="1">
-        <f t="array" ref="H4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1079,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="str" cm="1">
-        <f t="array" ref="H5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000000</v>
       </c>
       <c r="I5" s="1">
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="str" cm="1">
-        <f t="array" ref="H6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000000</v>
       </c>
       <c r="I6" s="1">
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="str" cm="1">
-        <f t="array" ref="H7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010011</v>
       </c>
       <c r="I7" s="1">
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="str" cm="1">
-        <f t="array" ref="H8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010011</v>
       </c>
       <c r="I8" s="1">
@@ -1318,7 +1318,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="str" cm="1">
-        <f t="array" ref="H9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010111</v>
       </c>
       <c r="I9" s="1">
@@ -1378,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="str" cm="1">
-        <f t="array" ref="H10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
       <c r="I10" s="1">
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="str" cm="1">
-        <f t="array" ref="H11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010110</v>
       </c>
       <c r="I11" s="1">
@@ -1497,7 +1497,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="str" cm="1">
-        <f t="array" ref="H12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010101</v>
       </c>
       <c r="I12" s="1">
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="1" t="str" cm="1">
-        <f t="array" ref="H13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010101</v>
       </c>
       <c r="I13" s="1">
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="str" cm="1">
-        <f t="array" ref="H14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010100</v>
       </c>
       <c r="I14" s="1">
@@ -1674,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="str" cm="1">
-        <f t="array" ref="H15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <f t="array" ref="H15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010100</v>
       </c>
       <c r="I15" s="1">
@@ -1715,7 +1715,7 @@
         <v>53</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>17</v>
@@ -1733,8 +1733,8 @@
         <v>0</v>
       </c>
       <c r="H16" s="1" t="str" cm="1">
-        <f t="array" ref="H16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>011000</v>
+        <f t="array" ref="H16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>111000</v>
       </c>
       <c r="I16" s="7">
         <v>0</v>
@@ -2781,7 +2781,7 @@
         <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>21</v>
@@ -2799,8 +2799,8 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="str" cm="1">
-        <f t="array" ref="H17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>011000</v>
+        <f t="array" ref="H17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>111000</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
new excel sheet uploaded
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alek\cpre_381\Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC44A7-BFB9-4489-8047-CF74577F1BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CD79BB3-E04D-44AC-A813-971EC8231E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38805" yWindow="-16515" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="105">
   <si>
     <t>Instruction</t>
   </si>
@@ -319,13 +319,67 @@
   </si>
   <si>
     <t>ALUControl (i_ALU_C) [6]</t>
+  </si>
+  <si>
+    <t>ALU Control Bits</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>[4]</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[0]</t>
+  </si>
+  <si>
+    <t>MUX Selector</t>
+  </si>
+  <si>
+    <t>Shift Logical Or Arith</t>
+  </si>
+  <si>
+    <t>Signed Or Unsigned</t>
+  </si>
+  <si>
+    <t>SLT Bit</t>
+  </si>
+  <si>
+    <t>"010100"</t>
+  </si>
+  <si>
+    <t>o_halt</t>
+  </si>
+  <si>
+    <t>halt</t>
+  </si>
+  <si>
+    <t>Tests Pass Or Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>fali</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -346,6 +400,26 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -361,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -384,11 +458,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,6 +587,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -827,38 +1018,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ39"/>
+  <dimension ref="A1:AMK39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.8125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.75" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.3125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.9375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.4375" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.8125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.8125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.9375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.6875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="25.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="22.8125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.25" style="3" customWidth="1"/>
-    <col min="12" max="12" width="27.5" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14.0625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.5" style="3" customWidth="1"/>
-    <col min="15" max="15" width="22.625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="14.0625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="21.9375" style="3" customWidth="1"/>
-    <col min="18" max="1024" width="10.8125" style="3"/>
+    <col min="5" max="6" width="21.8125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.9375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.6875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="22.8125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.25" style="3" customWidth="1"/>
+    <col min="13" max="13" width="27.5" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.0625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.5" style="3" customWidth="1"/>
+    <col min="16" max="16" width="22.625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.0625" style="3" customWidth="1"/>
+    <col min="18" max="19" width="21.9375" style="3" customWidth="1"/>
+    <col min="20" max="1025" width="10.8125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -874,10 +1065,9 @@
       <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="13"/>
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
@@ -887,51 +1077,58 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="S2" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -953,26 +1150,26 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="str" cm="1">
-        <f t="array" ref="H3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="str" cm="1">
+        <f t="array" ref="I3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
       <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="1" t="str">
-        <f t="shared" ref="L3:L25" si="0">IF(C3="R", "01", IF(C3="I", "00", IF(C3="J", "TODO", "")))</f>
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M26" si="0">IF(C3="R", "01", IF(C3="I", "00", IF(C3="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
@@ -985,8 +1182,14 @@
       <c r="Q3" s="1">
         <v>0</v>
       </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1006,42 +1209,48 @@
         <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1" t="str" cm="1">
-        <f t="array" ref="H4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I4" s="1" t="str" cm="1">
+        <f t="array" ref="I4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="1" t="str">
+      <c r="M4" s="1" t="str">
         <f>IF(C4="R", "01", IF(C4="I", "00", IF(C4="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="S4" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1061,42 +1270,48 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="str" cm="1">
-        <f t="array" ref="H5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I5" s="1" t="str" cm="1">
+        <f t="array" ref="I5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000000</v>
       </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
       <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="1" t="str">
+      <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
         <v>1</v>
       </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -1118,26 +1333,26 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="str" cm="1">
-        <f t="array" ref="H6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="str" cm="1">
+        <f t="array" ref="I6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000000</v>
       </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
       <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="L6" s="1" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
       <c r="N6" s="1">
         <v>0</v>
       </c>
@@ -1150,9 +1365,14 @@
       <c r="Q6" s="1">
         <v>0</v>
       </c>
-      <c r="R6" s="4"/>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1174,26 +1394,26 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="str" cm="1">
-        <f t="array" ref="H7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010011</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="str" cm="1">
+        <f t="array" ref="I7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000011</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>1</v>
       </c>
-      <c r="L7" s="1" t="str">
+      <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
@@ -1206,9 +1426,14 @@
       <c r="Q7" s="1">
         <v>0</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1228,43 +1453,48 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="str" cm="1">
-        <f t="array" ref="H8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010011</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
+      <c r="I8" s="1" t="str" cm="1">
+        <f t="array" ref="I8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000011</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
       <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
         <v>1</v>
       </c>
-      <c r="L8" s="1" t="str">
+      <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
       <c r="N8" s="1">
         <v>0</v>
       </c>
       <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
         <v>1</v>
       </c>
-      <c r="P8" s="1">
-        <v>0</v>
-      </c>
       <c r="Q8" s="1">
         <v>0</v>
       </c>
-      <c r="R8" s="4"/>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1284,28 +1514,28 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="str" cm="1">
-        <f t="array" ref="H9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I9" s="1" t="str" cm="1">
+        <f t="array" ref="I9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010111</v>
       </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
       <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>1</v>
       </c>
-      <c r="L9" s="1" t="str">
+      <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
       <c r="N9" s="1">
         <v>0</v>
       </c>
@@ -1318,9 +1548,14 @@
       <c r="Q9" s="1">
         <v>0</v>
       </c>
-      <c r="R9" s="4"/>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1340,43 +1575,48 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="1" t="str" cm="1">
-        <f t="array" ref="H10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I10" s="1" t="str" cm="1">
+        <f t="array" ref="I10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
       <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
         <v>1</v>
       </c>
-      <c r="L10" s="1" t="str">
+      <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M10" s="1">
-        <v>0</v>
-      </c>
       <c r="N10" s="1">
         <v>0</v>
       </c>
       <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
         <v>1</v>
       </c>
-      <c r="P10" s="1">
-        <v>0</v>
-      </c>
       <c r="Q10" s="1">
         <v>0</v>
       </c>
-      <c r="R10" s="4"/>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1398,26 +1638,26 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1" t="str" cm="1">
-        <f t="array" ref="H11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010110</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="str" cm="1">
+        <f t="array" ref="I11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000110</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
       <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
         <v>1</v>
       </c>
-      <c r="L11" s="1" t="str">
+      <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
       <c r="N11" s="1">
         <v>0</v>
       </c>
@@ -1430,8 +1670,14 @@
       <c r="Q11" s="1">
         <v>0</v>
       </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -1451,28 +1697,28 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="str" cm="1">
+        <f t="array" ref="I12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000101</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="1" t="str" cm="1">
-        <f t="array" ref="H12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010101</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="str">
+      <c r="M12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
@@ -1485,8 +1731,14 @@
       <c r="Q12" s="1">
         <v>0</v>
       </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -1506,42 +1758,48 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="H13" s="1" t="str" cm="1">
-        <f t="array" ref="H13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010101</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
+      <c r="I13" s="1" t="str" cm="1">
+        <f t="array" ref="I13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000101</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
         <v>1</v>
       </c>
-      <c r="L13" s="1" t="str">
+      <c r="M13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
       <c r="N13" s="1">
         <v>0</v>
       </c>
       <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
         <v>1</v>
       </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
       <c r="Q13" s="1">
         <v>0</v>
       </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1563,26 +1821,26 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1" t="str" cm="1">
-        <f t="array" ref="H14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010100</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="str" cm="1">
+        <f t="array" ref="I14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000100</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
       </c>
       <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
         <v>1</v>
       </c>
-      <c r="L14" s="1" t="str">
+      <c r="M14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
@@ -1595,8 +1853,14 @@
       <c r="Q14" s="1">
         <v>0</v>
       </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -1616,33 +1880,33 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="1" t="str" cm="1">
-        <f t="array" ref="H15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010100</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
+      <c r="I15" s="1" t="str" cm="1">
+        <f t="array" ref="I15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000100</v>
       </c>
       <c r="J15" s="1">
         <v>0</v>
       </c>
       <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
         <v>1</v>
       </c>
-      <c r="L15" s="1" t="str">
+      <c r="M15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
       <c r="N15" s="1">
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -1650,8 +1914,14 @@
       <c r="Q15" s="1">
         <v>0</v>
       </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="16" spans="1:1024" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:1025" s="9" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1673,40 +1943,44 @@
       <c r="G16" s="7">
         <v>0</v>
       </c>
-      <c r="H16" s="1" t="str" cm="1">
-        <f t="array" ref="H16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="str" cm="1">
+        <f t="array" ref="I16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>111000</v>
       </c>
-      <c r="I16" s="7">
-        <v>0</v>
-      </c>
       <c r="J16" s="7">
         <v>0</v>
       </c>
       <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
         <v>1</v>
       </c>
-      <c r="L16" s="7" t="str">
+      <c r="M16" s="7" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M16" s="7">
-        <v>0</v>
-      </c>
       <c r="N16" s="7">
         <v>0</v>
       </c>
       <c r="O16" s="7">
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
         <v>1</v>
       </c>
-      <c r="P16" s="7">
-        <v>0</v>
-      </c>
       <c r="Q16" s="7">
         <v>0</v>
       </c>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
+      <c r="R16" s="7">
+        <v>0</v>
+      </c>
+      <c r="S16" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
@@ -2712,8 +2986,9 @@
       <c r="AMH16" s="8"/>
       <c r="AMI16" s="8"/>
       <c r="AMJ16" s="8"/>
+      <c r="AMK16" s="8"/>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -2733,42 +3008,48 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="H17" s="1" t="str" cm="1">
-        <f t="array" ref="H17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I17" s="1" t="str" cm="1">
+        <f t="array" ref="I17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>111000</v>
       </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
       <c r="J17" s="1">
         <v>0</v>
       </c>
       <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" s="1" t="str">
+      <c r="M17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
       <c r="N17" s="1">
         <v>0</v>
       </c>
       <c r="O17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
         <v>1</v>
       </c>
-      <c r="P17" s="1">
-        <v>0</v>
-      </c>
       <c r="Q17" s="1">
         <v>0</v>
       </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -2788,42 +3069,48 @@
         <v>1</v>
       </c>
       <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="str" cm="1">
-        <f t="array" ref="H18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>010010</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="str" cm="1">
+        <f t="array" ref="I18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000010</v>
       </c>
       <c r="J18" s="1">
         <v>0</v>
       </c>
       <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
         <v>1</v>
       </c>
-      <c r="L18" s="1" t="str">
+      <c r="M18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M18" s="1">
-        <v>0</v>
-      </c>
       <c r="N18" s="1">
         <v>0</v>
       </c>
       <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
         <v>1</v>
       </c>
-      <c r="P18" s="1">
-        <v>0</v>
-      </c>
       <c r="Q18" s="1">
         <v>0</v>
       </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -2843,42 +3130,48 @@
         <v>1</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="str" cm="1">
-        <f t="array" ref="H19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>010001</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="str" cm="1">
+        <f t="array" ref="I19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000001</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
       </c>
       <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
         <v>1</v>
       </c>
-      <c r="L19" s="1" t="str">
+      <c r="M19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M19" s="1">
-        <v>0</v>
-      </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
         <v>1</v>
       </c>
-      <c r="P19" s="1">
-        <v>0</v>
-      </c>
       <c r="Q19" s="1">
         <v>0</v>
       </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+      <c r="S19" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="20" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:1025" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -2898,42 +3191,48 @@
         <v>1</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="str" cm="1">
-        <f t="array" ref="H20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>011001</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="str" cm="1">
+        <f t="array" ref="I20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>001001</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
         <v>1</v>
       </c>
-      <c r="L20" s="1" t="str">
+      <c r="M20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M20" s="1">
-        <v>0</v>
-      </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
         <v>1</v>
       </c>
-      <c r="P20" s="1">
-        <v>0</v>
-      </c>
       <c r="Q20" s="1">
         <v>0</v>
       </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2953,42 +3252,48 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="H21" s="1" t="str" cm="1">
-        <f t="array" ref="H21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I21" s="1" t="str" cm="1">
+        <f t="array" ref="I21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
       <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
         <v>1</v>
       </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
-      <c r="L21" s="6" t="str">
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
         <v>1</v>
       </c>
-      <c r="P21" s="1">
-        <v>0</v>
-      </c>
       <c r="Q21" s="1">
         <v>0</v>
       </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -3010,26 +3315,26 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1" t="str" cm="1">
-        <f t="array" ref="H22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="str" cm="1">
+        <f t="array" ref="I22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011000</v>
       </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
       <c r="J22" s="1">
         <v>0</v>
       </c>
       <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
         <v>1</v>
       </c>
-      <c r="L22" s="1" t="str">
+      <c r="M22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
       <c r="N22" s="1">
         <v>0</v>
       </c>
@@ -3042,8 +3347,14 @@
       <c r="Q22" s="1">
         <v>0</v>
       </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
@@ -3065,26 +3376,26 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="1" t="str" cm="1">
-        <f t="array" ref="H23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="str" cm="1">
+        <f t="array" ref="I23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>001000</v>
       </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
       <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
         <v>1</v>
       </c>
-      <c r="L23" s="1" t="str">
+      <c r="M23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="M23" s="1">
-        <v>0</v>
-      </c>
       <c r="N23" s="1">
         <v>0</v>
       </c>
@@ -3097,8 +3408,14 @@
       <c r="Q23" s="1">
         <v>0</v>
       </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -3118,42 +3435,48 @@
         <v>0</v>
       </c>
       <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
         <v>1</v>
       </c>
-      <c r="H24" s="1" t="str" cm="1">
-        <f t="array" ref="H24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I24" s="1" t="str" cm="1">
+        <f t="array" ref="I24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011000</v>
       </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
       <c r="J24" s="1">
         <v>0</v>
       </c>
       <c r="K24" s="1">
         <v>0</v>
       </c>
-      <c r="L24" s="1" t="str">
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M24" s="1">
-        <v>0</v>
-      </c>
       <c r="N24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="1">
         <v>1</v>
       </c>
       <c r="P24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="1">
         <v>0</v>
       </c>
+      <c r="R24" s="1">
+        <v>0</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -3173,42 +3496,48 @@
         <v>0</v>
       </c>
       <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="1" t="str" cm="1">
-        <f t="array" ref="H25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I25" s="1" t="str" cm="1">
+        <f t="array" ref="I25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011000</v>
       </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
       <c r="J25" s="1">
         <v>0</v>
       </c>
       <c r="K25" s="1">
         <v>0</v>
       </c>
-      <c r="L25" s="1" t="str">
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="M25" s="1">
-        <v>0</v>
-      </c>
       <c r="N25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1">
         <v>1</v>
       </c>
       <c r="P25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="1">
         <v>0</v>
       </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="26" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -3228,15 +3557,15 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
         <v>1</v>
       </c>
-      <c r="H26" s="1" t="str" cm="1">
-        <f t="array" ref="H26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I26" s="1" t="str" cm="1">
+        <f t="array" ref="I26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
       <c r="J26" s="1">
         <v>0</v>
       </c>
@@ -3246,12 +3575,13 @@
       <c r="L26" s="1">
         <v>0</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M26" s="1" t="str">
+        <f>IF(C26="R", "01", IF(C26="I", "00", IF(C26="J", "00", "")))</f>
+        <v>00</v>
+      </c>
+      <c r="N26" s="1">
         <v>1</v>
       </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
       <c r="O26" s="1">
         <v>0</v>
       </c>
@@ -3261,8 +3591,14 @@
       <c r="Q26" s="1">
         <v>0</v>
       </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3282,41 +3618,47 @@
         <v>0</v>
       </c>
       <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
         <v>1</v>
       </c>
-      <c r="H27" s="1" t="str" cm="1">
-        <f t="array" ref="H27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I27" s="1" t="str" cm="1">
+        <f t="array" ref="I27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
       <c r="J27" s="1">
         <v>0</v>
       </c>
       <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
         <v>1</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>11</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>1</v>
       </c>
-      <c r="N27" s="1">
-        <v>0</v>
-      </c>
       <c r="O27" s="1">
         <v>0</v>
       </c>
       <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
         <v>1</v>
       </c>
-      <c r="Q27" s="1">
-        <v>0</v>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:1025" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
@@ -3336,28 +3678,28 @@
         <v>1</v>
       </c>
       <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1" t="str" cm="1">
-        <f t="array" ref="H28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="str" cm="1">
+        <f t="array" ref="I28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
       <c r="J28" s="1">
         <v>0</v>
       </c>
       <c r="K28" s="1">
         <v>0</v>
       </c>
-      <c r="L28" s="1" t="str">
-        <f t="shared" ref="L28:L35" si="1">IF(C28="R", "01", IF(C28="I", "00", IF(C28="J", "TODO", "")))</f>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1" t="str">
+        <f t="shared" ref="M28:M35" si="1">IF(C28="R", "01", IF(C28="I", "00", IF(C28="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="M28" s="1">
-        <v>0</v>
-      </c>
       <c r="N28" s="1">
         <v>0</v>
       </c>
@@ -3368,10 +3710,16 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="R28" s="1">
         <v>1</v>
       </c>
+      <c r="S28" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="29" spans="1:1024" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:1025" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A29" s="6" t="s">
         <v>75</v>
       </c>
@@ -3391,28 +3739,28 @@
         <v>0</v>
       </c>
       <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
         <v>1</v>
       </c>
-      <c r="H29" s="6" t="str" cm="1">
-        <f t="array" ref="H29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I29" s="1" t="str" cm="1">
+        <f t="array" ref="I29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I29" s="6">
+      <c r="J29" s="6">
         <v>1</v>
       </c>
-      <c r="J29" s="6">
-        <v>0</v>
-      </c>
       <c r="K29" s="6">
+        <v>0</v>
+      </c>
+      <c r="L29" s="6">
         <v>1</v>
       </c>
-      <c r="L29" s="6" t="str">
+      <c r="M29" s="6" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-      <c r="M29" s="6">
-        <v>0</v>
-      </c>
       <c r="N29" s="6">
         <v>0</v>
       </c>
@@ -3425,8 +3773,12 @@
       <c r="Q29" s="6">
         <v>0</v>
       </c>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
+      <c r="R29" s="6">
+        <v>0</v>
+      </c>
+      <c r="S29" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
@@ -4432,8 +4784,9 @@
       <c r="AMH29" s="10"/>
       <c r="AMI29" s="10"/>
       <c r="AMJ29" s="10"/>
+      <c r="AMK29" s="10"/>
     </row>
-    <row r="30" spans="1:1024" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:1025" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A30" s="6" t="s">
         <v>76</v>
       </c>
@@ -4453,28 +4806,28 @@
         <v>0</v>
       </c>
       <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
         <v>1</v>
       </c>
-      <c r="H30" s="6" t="str" cm="1">
-        <f t="array" ref="H30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I30" s="1" t="str" cm="1">
+        <f t="array" ref="I30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I30" s="6">
+      <c r="J30" s="6">
         <v>1</v>
       </c>
-      <c r="J30" s="6">
-        <v>0</v>
-      </c>
       <c r="K30" s="6">
+        <v>0</v>
+      </c>
+      <c r="L30" s="6">
         <v>1</v>
       </c>
-      <c r="L30" s="6" t="str">
+      <c r="M30" s="6" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-      <c r="M30" s="6">
-        <v>0</v>
-      </c>
       <c r="N30" s="6">
         <v>0</v>
       </c>
@@ -4487,8 +4840,12 @@
       <c r="Q30" s="6">
         <v>0</v>
       </c>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
+      <c r="R30" s="6">
+        <v>0</v>
+      </c>
+      <c r="S30" s="22" t="s">
+        <v>104</v>
+      </c>
       <c r="T30" s="10"/>
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
@@ -5494,8 +5851,9 @@
       <c r="AMH30" s="10"/>
       <c r="AMI30" s="10"/>
       <c r="AMJ30" s="10"/>
+      <c r="AMK30" s="10"/>
     </row>
-    <row r="31" spans="1:1024" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:1025" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A31" s="6" t="s">
         <v>77</v>
       </c>
@@ -5515,28 +5873,28 @@
         <v>0</v>
       </c>
       <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6">
         <v>1</v>
       </c>
-      <c r="H31" s="6" t="str" cm="1">
-        <f t="array" ref="H31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I31" s="1" t="str" cm="1">
+        <f t="array" ref="I31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I31" s="6">
+      <c r="J31" s="6">
         <v>1</v>
       </c>
-      <c r="J31" s="6">
-        <v>0</v>
-      </c>
       <c r="K31" s="6">
+        <v>0</v>
+      </c>
+      <c r="L31" s="6">
         <v>1</v>
       </c>
-      <c r="L31" s="6" t="str">
+      <c r="M31" s="6" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-      <c r="M31" s="6">
-        <v>0</v>
-      </c>
       <c r="N31" s="6">
         <v>0</v>
       </c>
@@ -5549,8 +5907,12 @@
       <c r="Q31" s="6">
         <v>0</v>
       </c>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
+      <c r="R31" s="6">
+        <v>0</v>
+      </c>
+      <c r="S31" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="T31" s="10"/>
       <c r="U31" s="10"/>
       <c r="V31" s="10"/>
@@ -6556,8 +6918,9 @@
       <c r="AMH31" s="10"/>
       <c r="AMI31" s="10"/>
       <c r="AMJ31" s="10"/>
+      <c r="AMK31" s="10"/>
     </row>
-    <row r="32" spans="1:1024" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:1025" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A32" s="6" t="s">
         <v>78</v>
       </c>
@@ -6577,28 +6940,28 @@
         <v>0</v>
       </c>
       <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
         <v>1</v>
       </c>
-      <c r="H32" s="6" t="str" cm="1">
-        <f t="array" ref="H32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="I32" s="1" t="str" cm="1">
+        <f t="array" ref="I32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="I32" s="6">
+      <c r="J32" s="6">
         <v>1</v>
       </c>
-      <c r="J32" s="6">
-        <v>0</v>
-      </c>
       <c r="K32" s="6">
+        <v>0</v>
+      </c>
+      <c r="L32" s="6">
         <v>1</v>
       </c>
-      <c r="L32" s="6" t="str">
+      <c r="M32" s="6" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-      <c r="M32" s="6">
-        <v>0</v>
-      </c>
       <c r="N32" s="6">
         <v>0</v>
       </c>
@@ -6611,8 +6974,12 @@
       <c r="Q32" s="6">
         <v>0</v>
       </c>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
+      <c r="R32" s="6">
+        <v>0</v>
+      </c>
+      <c r="S32" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="T32" s="10"/>
       <c r="U32" s="10"/>
       <c r="V32" s="10"/>
@@ -7618,8 +7985,9 @@
       <c r="AMH32" s="10"/>
       <c r="AMI32" s="10"/>
       <c r="AMJ32" s="10"/>
+      <c r="AMK32" s="10"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>79</v>
       </c>
@@ -7641,26 +8009,26 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="1" t="str" cm="1">
-        <f t="array" ref="H33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>010010</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0</v>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="str" cm="1">
+        <f t="array" ref="I33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000010</v>
       </c>
       <c r="J33" s="1">
         <v>0</v>
       </c>
       <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
         <v>1</v>
       </c>
-      <c r="L33" s="1" t="str">
+      <c r="M33" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01</v>
       </c>
-      <c r="M33" s="1">
-        <v>0</v>
-      </c>
       <c r="N33" s="1">
         <v>0</v>
       </c>
@@ -7673,8 +8041,14 @@
       <c r="Q33" s="1">
         <v>0</v>
       </c>
+      <c r="R33" s="1">
+        <v>0</v>
+      </c>
+      <c r="S33" s="21" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
@@ -7696,26 +8070,26 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="1" t="str" cm="1">
-        <f t="array" ref="H34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
-        <v>010001</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="str" cm="1">
+        <f t="array" ref="I34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000001</v>
       </c>
       <c r="J34" s="1">
         <v>0</v>
       </c>
       <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
         <v>1</v>
       </c>
-      <c r="L34" s="1" t="str">
+      <c r="M34" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01</v>
       </c>
-      <c r="M34" s="1">
-        <v>0</v>
-      </c>
       <c r="N34" s="1">
         <v>0</v>
       </c>
@@ -7728,8 +8102,14 @@
       <c r="Q34" s="1">
         <v>0</v>
       </c>
+      <c r="R34" s="1">
+        <v>0</v>
+      </c>
+      <c r="S34" s="21" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
@@ -7751,26 +8131,26 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="1" t="str" cm="1">
-        <f t="array" ref="H35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "010011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111", "TODO")</f>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1" t="str" cm="1">
+        <f t="array" ref="I35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "000011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011001</v>
       </c>
-      <c r="I35" s="1">
-        <v>0</v>
-      </c>
       <c r="J35" s="1">
         <v>0</v>
       </c>
       <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
         <v>1</v>
       </c>
-      <c r="L35" s="1" t="str">
+      <c r="M35" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01</v>
       </c>
-      <c r="M35" s="1">
-        <v>0</v>
-      </c>
       <c r="N35" s="1">
         <v>0</v>
       </c>
@@ -7783,12 +8163,118 @@
       <c r="Q35" s="1">
         <v>0</v>
       </c>
+      <c r="R35" s="1">
+        <v>0</v>
+      </c>
+      <c r="S35" s="21" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="H38" s="4"/>
+    <row r="36" spans="1:19" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+      <c r="S36" s="21" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="H39" s="4"/>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="G37" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38" s="16"/>
+      <c r="H38" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="I39" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7796,7 +8282,7 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:Q1"/>
+    <mergeCell ref="H1:R1"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
lb and lbu work, need to finish load word and lwu
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -429,7 +429,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -471,6 +471,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4EA72E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -578,7 +584,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -623,7 +629,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,7 +637,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -739,11 +749,11 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F44" activeCellId="0" sqref="F44"/>
+      <selection pane="bottomRight" activeCell="S44" activeCellId="0" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2481,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="10" t="n">
         <v>0</v>
@@ -2490,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="11" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" s="12" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2560,7 @@
       <c r="R30" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="S30" s="11" t="s">
+      <c r="S30" s="13" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2612,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="S31" s="11" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,7 +2682,7 @@
       <c r="R32" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="S32" s="11" t="s">
+      <c r="S32" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2919,51 +2929,51 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="K37" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="L37" s="14" t="s">
+      <c r="L37" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="M37" s="15" t="s">
+      <c r="M37" s="16" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G38" s="16"/>
-      <c r="H38" s="17" t="s">
+      <c r="G38" s="17"/>
+      <c r="H38" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="I38" s="17" t="s">
+      <c r="I38" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="K38" s="17" t="s">
+      <c r="K38" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="L38" s="17" t="s">
+      <c r="L38" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="M38" s="18" t="s">
+      <c r="M38" s="19" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I39" s="19"/>
+      <c r="I39" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
added beq signal to decoder and w_beq to mips proc.
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="108">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Control Signals</t>
   </si>
   <si>
+    <t xml:space="preserve">o_beq</t>
+  </si>
+  <si>
     <t xml:space="preserve">o_halt</t>
   </si>
   <si>
@@ -253,13 +256,13 @@
     <t xml:space="preserve">"000100"</t>
   </si>
   <si>
+    <t xml:space="preserve">bne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"000101"</t>
+  </si>
+  <si>
     <t xml:space="preserve">fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"000101"</t>
   </si>
   <si>
     <t xml:space="preserve">j</t>
@@ -351,12 +354,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -375,19 +379,28 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF996600"/>
+      <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -396,12 +409,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF4EA72E"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -413,8 +428,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -425,8 +440,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -518,14 +533,14 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,11 +557,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,63 +569,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,10 +633,10 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Neutral" xfId="20"/>
-    <cellStyle name="Good" xfId="21"/>
-    <cellStyle name="Warning" xfId="22"/>
-    <cellStyle name="Bad" xfId="23"/>
+    <cellStyle name="Bad 4" xfId="20"/>
+    <cellStyle name="Good 2" xfId="21"/>
+    <cellStyle name="Neutral 1" xfId="22"/>
+    <cellStyle name="Warning 3" xfId="23"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -699,14 +706,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X22" activeCellId="0" sqref="X22"/>
+      <selection pane="bottomRight" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -715,20 +722,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="21.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="21.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="20" style="1" width="10.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="21.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="21.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="21" style="1" width="10.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,10 +754,10 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="2"/>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -760,6 +767,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -767,7 +775,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -809,22 +817,25 @@
       <c r="S2" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="T2" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>0</v>
@@ -835,26 +846,26 @@
       <c r="H3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="4" t="str">
-        <f aca="false" t="array" ref="I3:I3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="str">
+        <f aca="false" t="array" ref="J3:J3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>0</v>
+      <c r="K3" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4" t="str">
         <f aca="false">IF(C3="R", "01", IF(C3="I", "00", IF(C3="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N3" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O3" s="4" t="n">
         <v>0</v>
       </c>
@@ -867,41 +878,44 @@
       <c r="R3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>25</v>
+      <c r="S3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="7" t="str">
-        <f aca="false" t="array" ref="I4:I4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="7" t="str">
+        <f aca="false" t="array" ref="J4:J4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>32</v>
@@ -909,44 +923,47 @@
       <c r="L4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="7" t="str">
+      <c r="M4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="7" t="str">
         <f aca="false">IF(C4="R", "01", IF(C4="I", "00", IF(C4="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>0</v>
@@ -955,61 +972,64 @@
         <v>0</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4" t="str">
-        <f aca="false" t="array" ref="I5:I5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="str">
+        <f aca="false" t="array" ref="J5:J5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000000</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>0</v>
+      <c r="K5" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4" t="str">
         <f aca="false">IF(C5="R", "01", IF(C5="I", "00", IF(C5="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N5" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O5" s="4" t="n">
         <v>0</v>
       </c>
       <c r="P5" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>25</v>
+      <c r="S5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="7" t="n">
+        <v>41</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="7" t="n">
@@ -1018,26 +1038,26 @@
       <c r="H6" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="7" t="str">
-        <f aca="false" t="array" ref="I6:I6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f aca="false" t="array" ref="J6:J6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000000</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="7" t="n">
-        <v>0</v>
+      <c r="K6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7" t="str">
         <f aca="false">IF(C6="R", "01", IF(C6="I", "00", IF(C6="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N6" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O6" s="7" t="n">
         <v>0</v>
       </c>
@@ -1050,25 +1070,28 @@
       <c r="R6" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>25</v>
+      <c r="S6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>0</v>
@@ -1079,26 +1102,26 @@
       <c r="H7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="4" t="str">
-        <f aca="false" t="array" ref="I7:I7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4" t="str">
+        <f aca="false" t="array" ref="J7:J7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000011</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>0</v>
+      <c r="K7" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4" t="str">
         <f aca="false">IF(C7="R", "01", IF(C7="I", "00", IF(C7="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N7" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O7" s="4" t="n">
         <v>0</v>
       </c>
@@ -1111,86 +1134,92 @@
       <c r="R7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>25</v>
+      <c r="S7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F8" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7" t="str">
-        <f aca="false" t="array" ref="I8:I8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f aca="false" t="array" ref="J8:J8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000011</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="7" t="n">
-        <v>0</v>
+      <c r="K8" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7" t="str">
         <f aca="false">IF(C8="R", "01", IF(C8="I", "00", IF(C8="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N8" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="P8" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S8" s="5" t="s">
-        <v>25</v>
+      <c r="S8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>0</v>
@@ -1199,28 +1228,28 @@
         <v>0</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4" t="str">
-        <f aca="false" t="array" ref="I9:I9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4" t="str">
+        <f aca="false" t="array" ref="J9:J9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010111</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="4" t="n">
-        <v>0</v>
+      <c r="K9" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4" t="str">
         <f aca="false">IF(C9="R", "01", IF(C9="I", "00", IF(C9="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N9" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O9" s="4" t="n">
         <v>0</v>
       </c>
@@ -1233,86 +1262,92 @@
       <c r="R9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>25</v>
+      <c r="S9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="7" t="str">
-        <f aca="false" t="array" ref="I10:I10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7" t="str">
+        <f aca="false" t="array" ref="J10:J10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="7" t="n">
-        <v>0</v>
+      <c r="K10" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7" t="str">
         <f aca="false">IF(C10="R", "01", IF(C10="I", "00", IF(C10="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N10" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="P10" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S10" s="5" t="s">
-        <v>25</v>
+      <c r="S10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>0</v>
@@ -1323,26 +1358,26 @@
       <c r="H11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="4" t="str">
-        <f aca="false" t="array" ref="I11:I11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="str">
+        <f aca="false" t="array" ref="J11:J11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000110</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="4" t="n">
-        <v>0</v>
+      <c r="K11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4" t="str">
         <f aca="false">IF(C11="R", "01", IF(C11="I", "00", IF(C11="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N11" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O11" s="4" t="n">
         <v>0</v>
       </c>
@@ -1355,27 +1390,30 @@
       <c r="R11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S11" s="5" t="s">
-        <v>25</v>
+      <c r="S11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="n">
@@ -1384,26 +1422,26 @@
       <c r="H12" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="7" t="str">
-        <f aca="false" t="array" ref="I12:I12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f aca="false" t="array" ref="J12:J12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000101</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="7" t="n">
-        <v>0</v>
+      <c r="K12" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="7" t="str">
         <f aca="false">IF(C12="R", "01", IF(C12="I", "00", IF(C12="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N12" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O12" s="7" t="n">
         <v>0</v>
       </c>
@@ -1416,25 +1454,28 @@
       <c r="R12" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S12" s="5" t="s">
-        <v>25</v>
+      <c r="S12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>0</v>
@@ -1443,61 +1484,64 @@
         <v>0</v>
       </c>
       <c r="H13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4" t="str">
-        <f aca="false" t="array" ref="I13:I13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4" t="str">
+        <f aca="false" t="array" ref="J13:J13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000101</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="4" t="n">
-        <v>0</v>
+      <c r="K13" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4" t="str">
         <f aca="false">IF(C13="R", "01", IF(C13="I", "00", IF(C13="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N13" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O13" s="4" t="n">
         <v>0</v>
       </c>
       <c r="P13" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S13" s="5" t="s">
-        <v>25</v>
+      <c r="S13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="F14" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="7" t="n">
@@ -1506,26 +1550,26 @@
       <c r="H14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="7" t="str">
-        <f aca="false" t="array" ref="I14:I14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7" t="str">
+        <f aca="false" t="array" ref="J14:J14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000100</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="7" t="n">
-        <v>0</v>
+      <c r="K14" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M14" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7" t="str">
         <f aca="false">IF(C14="R", "01", IF(C14="I", "00", IF(C14="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N14" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O14" s="7" t="n">
         <v>0</v>
       </c>
@@ -1538,25 +1582,28 @@
       <c r="R14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S14" s="5" t="s">
-        <v>25</v>
+      <c r="S14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>0</v>
@@ -1565,28 +1612,28 @@
         <v>0</v>
       </c>
       <c r="H15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="4" t="str">
-        <f aca="false" t="array" ref="I15:I15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4" t="str">
+        <f aca="false" t="array" ref="J15:J15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000100</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="4" t="n">
-        <v>0</v>
+      <c r="K15" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="4" t="str">
         <f aca="false">IF(C15="R", "01", IF(C15="I", "00", IF(C15="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N15" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O15" s="4" t="n">
         <v>0</v>
       </c>
@@ -1599,86 +1646,92 @@
       <c r="R15" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="S15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="7" t="str">
+        <f aca="false" t="array" ref="J16:J16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>111000</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7" t="str">
-        <f aca="false" t="array" ref="I16:I16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>111000</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M16" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="7" t="str">
         <f aca="false">IF(C16="R", "01", IF(C16="I", "00", IF(C16="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N16" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="P16" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S16" s="5" t="s">
-        <v>25</v>
+      <c r="S16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>0</v>
@@ -1687,242 +1740,254 @@
         <v>0</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="4" t="str">
-        <f aca="false" t="array" ref="I17:I17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f aca="false" t="array" ref="J17:J17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>111000</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="4" t="n">
-        <v>0</v>
+      <c r="K17" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4" t="str">
         <f aca="false">IF(C17="R", "01", IF(C17="I", "00", IF(C17="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N17" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O17" s="4" t="n">
         <v>0</v>
       </c>
       <c r="P17" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S17" s="5" t="s">
-        <v>25</v>
+      <c r="S17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="7" t="n">
+        <v>66</v>
+      </c>
+      <c r="F18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="7" t="str">
-        <f aca="false" t="array" ref="I18:I18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="7" t="str">
+        <f aca="false" t="array" ref="J18:J18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000010</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="7" t="n">
-        <v>0</v>
+      <c r="K18" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L18" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="7" t="str">
         <f aca="false">IF(C18="R", "01", IF(C18="I", "00", IF(C18="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N18" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="P18" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S18" s="5" t="s">
-        <v>25</v>
+      <c r="S18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4" t="str">
-        <f aca="false" t="array" ref="I19:I19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4" t="str">
+        <f aca="false" t="array" ref="J19:J19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000001</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="4" t="n">
-        <v>0</v>
+      <c r="K19" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M19" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4" t="str">
         <f aca="false">IF(C19="R", "01", IF(C19="I", "00", IF(C19="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N19" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O19" s="4" t="n">
         <v>0</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S19" s="5" t="s">
-        <v>25</v>
+      <c r="S19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7" t="str">
-        <f aca="false" t="array" ref="I20:I20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7" t="str">
+        <f aca="false" t="array" ref="J20:J20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>001001</v>
       </c>
-      <c r="J20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="7" t="n">
-        <v>0</v>
+      <c r="K20" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M20" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="7" t="str">
         <f aca="false">IF(C20="R", "01", IF(C20="I", "00", IF(C20="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N20" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="P20" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S20" s="5" t="s">
-        <v>25</v>
+      <c r="S20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>0</v>
@@ -1931,61 +1996,64 @@
         <v>0</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="4" t="str">
-        <f aca="false" t="array" ref="I21:I21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4" t="str">
+        <f aca="false" t="array" ref="J21:J21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="4" t="n">
-        <v>1</v>
+      <c r="K21" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="11" t="str">
         <f aca="false">IF(C21="R", "01", IF(C21="I", "00", IF(C21="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N21" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="P21" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S21" s="5" t="s">
-        <v>25</v>
+      <c r="S21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="7" t="n">
+        <v>74</v>
+      </c>
+      <c r="F22" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="7" t="n">
@@ -1994,26 +2062,26 @@
       <c r="H22" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="7" t="str">
-        <f aca="false" t="array" ref="I22:I22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="7" t="str">
+        <f aca="false" t="array" ref="J22:J22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011000</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="7" t="n">
-        <v>0</v>
+      <c r="K22" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L22" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M22" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M22" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" s="7" t="str">
         <f aca="false">IF(C22="R", "01", IF(C22="I", "00", IF(C22="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N22" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O22" s="7" t="n">
         <v>0</v>
       </c>
@@ -2026,25 +2094,28 @@
       <c r="R22" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S22" s="5" t="s">
-        <v>25</v>
+      <c r="S22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F23" s="4" t="n">
         <v>0</v>
@@ -2055,26 +2126,26 @@
       <c r="H23" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="4" t="str">
-        <f aca="false" t="array" ref="I23:I23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="str">
+        <f aca="false" t="array" ref="J23:J23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>001000</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="4" t="n">
-        <v>0</v>
+      <c r="K23" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M23" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="4" t="str">
         <f aca="false">IF(C23="R", "01", IF(C23="I", "00", IF(C23="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N23" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O23" s="4" t="n">
         <v>0</v>
       </c>
@@ -2087,28 +2158,31 @@
       <c r="R23" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S23" s="5" t="s">
-        <v>25</v>
+      <c r="S23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="7" t="n">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>1</v>
       </c>
       <c r="G24" s="7" t="n">
         <v>0</v>
@@ -2116,26 +2190,26 @@
       <c r="H24" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="7" t="str">
-        <f aca="false" t="array" ref="I24:I24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="7" t="str">
+        <f aca="false" t="array" ref="J24:J24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011000</v>
       </c>
-      <c r="J24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" s="7" t="n">
-        <v>0</v>
+      <c r="K24" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L24" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="M24" s="7" t="str">
+      <c r="M24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="7" t="str">
         <f aca="false">IF(C24="R", "01", IF(C24="I", "00", IF(C24="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N24" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O24" s="7" t="n">
         <v>1</v>
       </c>
@@ -2148,8 +2222,11 @@
       <c r="R24" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S24" s="11" t="s">
-        <v>77</v>
+      <c r="S24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,16 +2234,16 @@
         <v>78</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>0</v>
@@ -2177,31 +2254,31 @@
       <c r="H25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="4" t="str">
-        <f aca="false" t="array" ref="I25:I25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="str">
+        <f aca="false" t="array" ref="J25:J25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011000</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" s="4" t="n">
-        <v>0</v>
+      <c r="K25" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="4" t="str">
+      <c r="M25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4" t="str">
         <f aca="false">IF(C25="R", "01", IF(C25="I", "00", IF(C25="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N25" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O25" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="4" t="n">
         <v>0</v>
@@ -2209,57 +2286,60 @@
       <c r="R25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S25" s="5" t="s">
-        <v>25</v>
+      <c r="S25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="26" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F26" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="7" t="str">
-        <f aca="false" t="array" ref="I26:I26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="7" t="str">
+        <f aca="false" t="array" ref="J26:J26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J26" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K26" s="7" t="n">
-        <v>0</v>
+      <c r="K26" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L26" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="M26" s="7" t="str">
+      <c r="M26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7" t="str">
         <f aca="false">IF(C26="R", "01", IF(C26="I", "00", IF(C26="J", "00", "")))</f>
         <v>00</v>
       </c>
-      <c r="N26" s="7" t="n">
-        <v>1</v>
-      </c>
       <c r="O26" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="7" t="n">
         <v>0</v>
@@ -2270,25 +2350,28 @@
       <c r="R26" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S26" s="5" t="s">
-        <v>25</v>
+      <c r="S26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>0</v>
@@ -2297,88 +2380,91 @@
         <v>0</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I27" s="4" t="str">
-        <f aca="false" t="array" ref="I27:I27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" s="4" t="str">
+        <f aca="false" t="array" ref="J27:J27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="4" t="n">
-        <v>0</v>
+      <c r="K27" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L27" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="N27" s="4" t="n">
-        <v>1</v>
-      </c>
       <c r="O27" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="4" t="n">
         <v>0</v>
       </c>
       <c r="Q27" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S27" s="11" t="s">
-        <v>77</v>
+        <v>1</v>
+      </c>
+      <c r="S27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="7" t="n">
+        <v>29</v>
+      </c>
+      <c r="F28" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="7" t="str">
-        <f aca="false" t="array" ref="I28:I28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7" t="str">
+        <f aca="false" t="array" ref="J28:J28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K28" s="7" t="n">
-        <v>0</v>
+      <c r="K28" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L28" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="M28" s="7" t="str">
+      <c r="M28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7" t="str">
         <f aca="false">IF(C28="R", "01", IF(C28="I", "00", IF(C28="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N28" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O28" s="7" t="n">
         <v>0</v>
       </c>
@@ -2389,149 +2475,158 @@
         <v>0</v>
       </c>
       <c r="R28" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="S28" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I29" s="4" t="str">
-        <f aca="false" t="array" ref="I29:I29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="4" t="str">
+        <f aca="false" t="array" ref="J29:J29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K29" s="4" t="n">
-        <v>0</v>
+      <c r="K29" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="L29" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M29" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" s="4" t="str">
         <f aca="false">IF(C29="R", "01", IF(C29="I", "00", IF(C29="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N29" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O29" s="4" t="n">
         <v>0</v>
       </c>
       <c r="P29" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S29" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I30" s="14" t="str">
-        <f aca="false" t="array" ref="I30:I30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="S29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="7" t="str">
+        <f aca="false" t="array" ref="J30:J30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J30" s="14" t="n">
+      <c r="K30" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="K30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="M30" s="14" t="str">
+      <c r="L30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" s="7" t="str">
         <f aca="false">IF(C30="R", "01", IF(C30="I", "00", IF(C30="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>22</v>
+      <c r="O30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="F31" s="4" t="n">
         <v>0</v>
@@ -2540,28 +2635,28 @@
         <v>0</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I31" s="4" t="str">
-        <f aca="false" t="array" ref="I31:I31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4" t="str">
+        <f aca="false" t="array" ref="J31:J31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J31" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K31" s="4" t="n">
-        <v>0</v>
+      <c r="K31" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="L31" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M31" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" s="4" t="str">
         <f aca="false">IF(C31="R", "01", IF(C31="I", "00", IF(C31="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N31" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O31" s="4" t="n">
         <v>0</v>
       </c>
@@ -2574,86 +2669,92 @@
       <c r="R31" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S31" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" s="14" t="str">
-        <f aca="false" t="array" ref="I32:I32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="S31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" s="7" t="str">
+        <f aca="false" t="array" ref="J32:J32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>010000</v>
       </c>
-      <c r="J32" s="14" t="n">
+      <c r="K32" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="K32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="M32" s="14" t="str">
+      <c r="L32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" s="7" t="str">
         <f aca="false">IF(C32="R", "01", IF(C32="I", "00", IF(C32="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="N32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S32" s="5" t="s">
-        <v>25</v>
+      <c r="O32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="33" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>0</v>
@@ -2664,26 +2765,26 @@
       <c r="H33" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="4" t="str">
-        <f aca="false" t="array" ref="I33:I33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4" t="str">
+        <f aca="false" t="array" ref="J33:J33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000010</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="4" t="n">
-        <v>0</v>
+      <c r="K33" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L33" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M33" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" s="4" t="str">
         <f aca="false">IF(C33="R", "01", IF(C33="I", "00", IF(C33="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N33" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O33" s="4" t="n">
         <v>0</v>
       </c>
@@ -2696,27 +2797,30 @@
       <c r="R33" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S33" s="5" t="s">
-        <v>25</v>
+      <c r="S33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="7" t="n">
+        <v>92</v>
+      </c>
+      <c r="F34" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="7" t="n">
@@ -2725,26 +2829,26 @@
       <c r="H34" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I34" s="7" t="str">
-        <f aca="false" t="array" ref="I34:I34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7" t="str">
+        <f aca="false" t="array" ref="J34:J34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>000001</v>
       </c>
-      <c r="J34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K34" s="7" t="n">
-        <v>0</v>
+      <c r="K34" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L34" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M34" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="M34" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" s="7" t="str">
         <f aca="false">IF(C34="R", "01", IF(C34="I", "00", IF(C34="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N34" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="O34" s="7" t="n">
         <v>0</v>
       </c>
@@ -2757,25 +2861,28 @@
       <c r="R34" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S34" s="5" t="s">
-        <v>25</v>
+      <c r="S34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="35" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F35" s="4" t="n">
         <v>0</v>
@@ -2786,26 +2893,26 @@
       <c r="H35" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I35" s="4" t="str">
-        <f aca="false" t="array" ref="I35:I35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "000011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+      <c r="I35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="4" t="str">
+        <f aca="false" t="array" ref="J35:J35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "000011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
         <v>011001</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K35" s="4" t="n">
-        <v>0</v>
+      <c r="K35" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="L35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M35" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" s="4" t="str">
         <f aca="false">IF(C35="R", "01", IF(C35="I", "00", IF(C35="J", "TODO", "")))</f>
         <v>01</v>
       </c>
-      <c r="N35" s="4" t="n">
-        <v>0</v>
-      </c>
       <c r="O35" s="4" t="n">
         <v>0</v>
       </c>
@@ -2818,31 +2925,34 @@
       <c r="R35" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S35" s="5" t="s">
-        <v>25</v>
+      <c r="S35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="7" t="n">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="F36" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="7" t="n">
         <v>0</v>
@@ -2850,11 +2960,11 @@
       <c r="I36" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J36" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="7" t="n">
-        <v>0</v>
+      <c r="J36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L36" s="7" t="n">
         <v>0</v>
@@ -2877,8 +2987,11 @@
       <c r="R36" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="S36" s="5" t="s">
-        <v>25</v>
+      <c r="S36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,54 +3013,55 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="15"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G38" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="I38" s="17" t="s">
+      <c r="I38" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="K38" s="17" t="s">
+      <c r="K38" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="L38" s="17" t="s">
+      <c r="L38" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="M38" s="18" t="s">
+      <c r="M38" s="15" t="s">
         <v>102</v>
       </c>
+      <c r="N38" s="16" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G39" s="19"/>
-      <c r="H39" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="I39" s="20" t="s">
+      <c r="H39" s="17"/>
+      <c r="I39" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="J39" s="20" t="s">
+      <c r="J39" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="K39" s="20" t="s">
+      <c r="K39" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="L39" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="M39" s="21" t="s">
-        <v>106</v>
+      <c r="L39" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I40" s="22"/>
+      <c r="J40" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2956,7 +3070,7 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="I1:S1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
cleaning up some files
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="111">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">ALUSrc (i_ALU_src) [1]</t>
   </si>
   <si>
-    <t xml:space="preserve">ALUControl (i_ALU_C) [6]</t>
+    <t xml:space="preserve">ALUControl (i_ALU_C) [8]</t>
   </si>
   <si>
     <t xml:space="preserve">o_MemToReg [2]</t>
@@ -316,6 +316,12 @@
     <t xml:space="preserve">ALU Control Bits</t>
   </si>
   <si>
+    <t xml:space="preserve">[7]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[6]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[5]</t>
   </si>
   <si>
@@ -332,6 +338,9 @@
   </si>
   <si>
     <t xml:space="preserve">[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">branch</t>
   </si>
   <si>
     <t xml:space="preserve">SLT Bit</t>
@@ -354,7 +363,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -397,12 +406,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -540,7 +543,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -573,15 +576,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -593,7 +592,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -713,7 +712,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K19" activeCellId="0" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -850,8 +849,8 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f aca="false" t="array" ref="J3:J3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+        <f aca="false">_xlfn.SWITCH(B3, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>25</v>
@@ -901,7 +900,7 @@
       <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -913,9 +912,9 @@
       <c r="I4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="7" t="str">
-        <f aca="false" t="array" ref="J4:J4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+      <c r="J4" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B4, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>32</v>
@@ -930,7 +929,7 @@
         <f aca="false">IF(C4="R", "01", IF(C4="I", "00", IF(C4="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="8" t="s">
         <v>35</v>
       </c>
       <c r="P4" s="7" t="s">
@@ -978,8 +977,8 @@
         <v>1</v>
       </c>
       <c r="J5" s="4" t="str">
-        <f aca="false" t="array" ref="J5:J5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000000</v>
+        <f aca="false">_xlfn.SWITCH(B5, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000000</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>25</v>
@@ -1029,7 +1028,7 @@
       <c r="E6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="7" t="n">
@@ -1041,9 +1040,9 @@
       <c r="I6" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="7" t="str">
-        <f aca="false" t="array" ref="J6:J6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000000</v>
+      <c r="J6" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B6, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000000</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>25</v>
@@ -1106,8 +1105,8 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="str">
-        <f aca="false" t="array" ref="J7:J7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000011</v>
+        <f aca="false">_xlfn.SWITCH(B7, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000011</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>25</v>
@@ -1157,7 +1156,7 @@
       <c r="E8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="7" t="n">
@@ -1169,9 +1168,9 @@
       <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="7" t="str">
-        <f aca="false" t="array" ref="J8:J8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000011</v>
+      <c r="J8" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B8, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000011</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>25</v>
@@ -1234,8 +1233,8 @@
         <v>1</v>
       </c>
       <c r="J9" s="4" t="str">
-        <f aca="false" t="array" ref="J9:J9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010111</v>
+        <f aca="false">_xlfn.SWITCH(B9, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010111</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>25</v>
@@ -1285,7 +1284,7 @@
       <c r="E10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="7" t="n">
@@ -1297,9 +1296,9 @@
       <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="7" t="str">
-        <f aca="false" t="array" ref="J10:J10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+      <c r="J10" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B10, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>50</v>
@@ -1362,8 +1361,8 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="str">
-        <f aca="false" t="array" ref="J11:J11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000110</v>
+        <f aca="false">_xlfn.SWITCH(B11, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000110</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>25</v>
@@ -1413,7 +1412,7 @@
       <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="n">
@@ -1425,9 +1424,9 @@
       <c r="I12" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="7" t="str">
-        <f aca="false" t="array" ref="J12:J12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000101</v>
+      <c r="J12" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B12, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000101</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>25</v>
@@ -1490,8 +1489,8 @@
         <v>1</v>
       </c>
       <c r="J13" s="4" t="str">
-        <f aca="false" t="array" ref="J13:J13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000101</v>
+        <f aca="false">_xlfn.SWITCH(B13, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000101</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>25</v>
@@ -1541,7 +1540,7 @@
       <c r="E14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="7" t="n">
@@ -1553,9 +1552,9 @@
       <c r="I14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J14" s="7" t="str">
-        <f aca="false" t="array" ref="J14:J14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000100</v>
+      <c r="J14" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B14, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000100</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>25</v>
@@ -1618,8 +1617,8 @@
         <v>1</v>
       </c>
       <c r="J15" s="4" t="str">
-        <f aca="false" t="array" ref="J15:J15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000100</v>
+        <f aca="false">_xlfn.SWITCH(B15, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000100</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>25</v>
@@ -1653,7 +1652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>61</v>
       </c>
@@ -1669,7 +1668,7 @@
       <c r="E16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="7" t="n">
@@ -1681,9 +1680,9 @@
       <c r="I16" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="7" t="str">
-        <f aca="false" t="array" ref="J16:J16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>111000</v>
+      <c r="J16" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B16, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00111000</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>25</v>
@@ -1746,8 +1745,8 @@
         <v>1</v>
       </c>
       <c r="J17" s="4" t="str">
-        <f aca="false" t="array" ref="J17:J17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>111000</v>
+        <f aca="false">_xlfn.SWITCH(B17, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00111000</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>25</v>
@@ -1797,7 +1796,7 @@
       <c r="E18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="8" t="n">
+      <c r="F18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="7" t="n">
@@ -1809,9 +1808,9 @@
       <c r="I18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J18" s="7" t="str">
-        <f aca="false" t="array" ref="J18:J18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000010</v>
+      <c r="J18" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B18, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000010</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>25</v>
@@ -1874,8 +1873,8 @@
         <v>0</v>
       </c>
       <c r="J19" s="4" t="str">
-        <f aca="false" t="array" ref="J19:J19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000001</v>
+        <f aca="false">_xlfn.SWITCH(B19, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000001</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>25</v>
@@ -1925,7 +1924,7 @@
       <c r="E20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="8" t="n">
+      <c r="F20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="7" t="n">
@@ -1937,9 +1936,9 @@
       <c r="I20" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J20" s="7" t="str">
-        <f aca="false" t="array" ref="J20:J20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>001001</v>
+      <c r="J20" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B20, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00001001</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>25</v>
@@ -2002,8 +2001,8 @@
         <v>1</v>
       </c>
       <c r="J21" s="4" t="str">
-        <f aca="false" t="array" ref="J21:J21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+        <f aca="false">_xlfn.SWITCH(B21, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>25</v>
@@ -2014,7 +2013,7 @@
       <c r="M21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="N21" s="11" t="str">
+      <c r="N21" s="10" t="str">
         <f aca="false">IF(C21="R", "01", IF(C21="I", "00", IF(C21="J", "TODO", "")))</f>
         <v>00</v>
       </c>
@@ -2053,7 +2052,7 @@
       <c r="E22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="8" t="n">
+      <c r="F22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="7" t="n">
@@ -2065,9 +2064,9 @@
       <c r="I22" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J22" s="7" t="str">
-        <f aca="false" t="array" ref="J22:J22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>011000</v>
+      <c r="J22" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B22, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00011000</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>25</v>
@@ -2130,8 +2129,8 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="str">
-        <f aca="false" t="array" ref="J23:J23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>001000</v>
+        <f aca="false">_xlfn.SWITCH(B23, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00001000</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>25</v>
@@ -2181,7 +2180,7 @@
       <c r="E24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="8" t="n">
+      <c r="F24" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G24" s="7" t="n">
@@ -2193,9 +2192,9 @@
       <c r="I24" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J24" s="7" t="str">
-        <f aca="false" t="array" ref="J24:J24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>011000</v>
+      <c r="J24" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B24, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00011000</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>25</v>
@@ -2258,8 +2257,8 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f aca="false" t="array" ref="J25:J25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>011000</v>
+        <f aca="false">_xlfn.SWITCH(B25, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00011000</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>25</v>
@@ -2289,7 +2288,7 @@
       <c r="S25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="T25" s="12" t="s">
+      <c r="T25" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2309,7 +2308,7 @@
       <c r="E26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="8" t="n">
+      <c r="F26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="7" t="n">
@@ -2321,9 +2320,9 @@
       <c r="I26" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J26" s="7" t="str">
-        <f aca="false" t="array" ref="J26:J26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+      <c r="J26" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B26, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>25</v>
@@ -2353,7 +2352,7 @@
       <c r="S26" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="T26" s="12" t="s">
+      <c r="T26" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2386,8 +2385,8 @@
         <v>1</v>
       </c>
       <c r="J27" s="4" t="str">
-        <f aca="false" t="array" ref="J27:J27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+        <f aca="false">_xlfn.SWITCH(B27, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>25</v>
@@ -2416,7 +2415,7 @@
       <c r="S27" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="T27" s="12" t="s">
+      <c r="T27" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2436,7 +2435,7 @@
       <c r="E28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="8" t="n">
+      <c r="F28" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="7" t="n">
@@ -2448,9 +2447,9 @@
       <c r="I28" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J28" s="7" t="str">
-        <f aca="false" t="array" ref="J28:J28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+      <c r="J28" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B28, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>25</v>
@@ -2480,41 +2479,41 @@
       <c r="S28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T28" s="12" t="s">
+      <c r="T28" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="29" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="11" t="n">
+      <c r="G29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10" t="n">
         <v>1</v>
       </c>
       <c r="J29" s="4" t="str">
-        <f aca="false" t="array" ref="J29:J29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+        <f aca="false">_xlfn.SWITCH(B29, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>86</v>
@@ -2564,7 +2563,7 @@
       <c r="E30" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="8" t="n">
+      <c r="F30" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="7" t="n">
@@ -2576,9 +2575,9 @@
       <c r="I30" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J30" s="7" t="str">
-        <f aca="false" t="array" ref="J30:J30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+      <c r="J30" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B30, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K30" s="7" t="n">
         <v>10</v>
@@ -2613,19 +2612,19 @@
       </c>
     </row>
     <row r="31" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F31" s="4" t="n">
@@ -2641,8 +2640,8 @@
         <v>1</v>
       </c>
       <c r="J31" s="4" t="str">
-        <f aca="false" t="array" ref="J31:J31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+        <f aca="false">_xlfn.SWITCH(B31, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>86</v>
@@ -2692,7 +2691,7 @@
       <c r="E32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="8" t="n">
+      <c r="F32" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="7" t="n">
@@ -2704,9 +2703,9 @@
       <c r="I32" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J32" s="7" t="str">
-        <f aca="false" t="array" ref="J32:J32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>010000</v>
+      <c r="J32" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B32, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00010000</v>
       </c>
       <c r="K32" s="7" t="n">
         <v>10</v>
@@ -2769,8 +2768,8 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="str">
-        <f aca="false" t="array" ref="J33:J33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000010</v>
+        <f aca="false">_xlfn.SWITCH(B33, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000010</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>25</v>
@@ -2820,7 +2819,7 @@
       <c r="E34" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="8" t="n">
+      <c r="F34" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="7" t="n">
@@ -2832,9 +2831,9 @@
       <c r="I34" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J34" s="7" t="str">
-        <f aca="false" t="array" ref="J34:J34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>000001</v>
+      <c r="J34" s="4" t="str">
+        <f aca="false">_xlfn.SWITCH(B34, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00000001</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>25</v>
@@ -2897,8 +2896,8 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="str">
-        <f aca="false" t="array" ref="J35:J35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "000011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
-        <v>011001</v>
+        <f aca="false">_xlfn.SWITCH(B35, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
+        <v>00001001</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>25</v>
@@ -2948,7 +2947,7 @@
       <c r="E36" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="8" t="n">
+      <c r="F36" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G36" s="7" t="n">
@@ -3014,54 +3013,68 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
-      <c r="T37" s="13"/>
+      <c r="T37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="14" t="s">
+      <c r="F38" s="0"/>
+      <c r="G38" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="I38" s="15" t="s">
+      <c r="H38" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="J38" s="15" t="s">
+      <c r="I38" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="J38" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="L38" s="15" t="s">
+      <c r="K38" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="M38" s="15" t="s">
+      <c r="L38" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="N38" s="16" t="s">
+      <c r="M38" s="14" t="s">
         <v>103</v>
       </c>
+      <c r="N38" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="17"/>
-      <c r="I39" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="K39" s="18" t="s">
+      <c r="F39" s="0"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="L39" s="18" t="s">
+      <c r="J39" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="M39" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="N39" s="19" t="s">
-        <v>107</v>
+      <c r="K39" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="N39" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="O39" s="18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="20"/>
+      <c r="J40" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Revert "cleaning up some files"
This reverts commit 0d0cef9611065d63c9a5d244c183a3589839619e
</commit_message>
<xml_diff>
--- a/Project1/Proj1_control_signals.xlsx
+++ b/Project1/Proj1_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="108">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">ALUSrc (i_ALU_src) [1]</t>
   </si>
   <si>
-    <t xml:space="preserve">ALUControl (i_ALU_C) [8]</t>
+    <t xml:space="preserve">ALUControl (i_ALU_C) [6]</t>
   </si>
   <si>
     <t xml:space="preserve">o_MemToReg [2]</t>
@@ -316,12 +316,6 @@
     <t xml:space="preserve">ALU Control Bits</t>
   </si>
   <si>
-    <t xml:space="preserve">[7]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[6]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[5]</t>
   </si>
   <si>
@@ -338,9 +332,6 @@
   </si>
   <si>
     <t xml:space="preserve">[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">branch</t>
   </si>
   <si>
     <t xml:space="preserve">SLT Bit</t>
@@ -363,7 +354,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -406,6 +397,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -543,7 +540,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -576,11 +573,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -592,7 +593,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -712,7 +713,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J44" activeCellId="0" sqref="J44"/>
+      <selection pane="bottomRight" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -849,8 +850,8 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B3, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+        <f aca="false" t="array" ref="J3:J3">_xlfn.SWITCH(B3, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>25</v>
@@ -900,7 +901,7 @@
       <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -912,9 +913,9 @@
       <c r="I4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B4, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+      <c r="J4" s="7" t="str">
+        <f aca="false" t="array" ref="J4:J4">_xlfn.SWITCH(B4, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>32</v>
@@ -929,7 +930,7 @@
         <f aca="false">IF(C4="R", "01", IF(C4="I", "00", IF(C4="J", "TODO", "")))</f>
         <v>00</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="P4" s="7" t="s">
@@ -977,8 +978,8 @@
         <v>1</v>
       </c>
       <c r="J5" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B5, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000000</v>
+        <f aca="false" t="array" ref="J5:J5">_xlfn.SWITCH(B5, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000000</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>25</v>
@@ -1028,7 +1029,7 @@
       <c r="E6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="7" t="n">
@@ -1040,9 +1041,9 @@
       <c r="I6" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B6, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000000</v>
+      <c r="J6" s="7" t="str">
+        <f aca="false" t="array" ref="J6:J6">_xlfn.SWITCH(B6, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000000</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>25</v>
@@ -1105,8 +1106,8 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B7, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000011</v>
+        <f aca="false" t="array" ref="J7:J7">_xlfn.SWITCH(B7, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000011</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>25</v>
@@ -1156,7 +1157,7 @@
       <c r="E8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="7" t="n">
@@ -1168,9 +1169,9 @@
       <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B8, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000011</v>
+      <c r="J8" s="7" t="str">
+        <f aca="false" t="array" ref="J8:J8">_xlfn.SWITCH(B8, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000011</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>25</v>
@@ -1233,8 +1234,8 @@
         <v>1</v>
       </c>
       <c r="J9" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B9, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010111</v>
+        <f aca="false" t="array" ref="J9:J9">_xlfn.SWITCH(B9, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010111</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>25</v>
@@ -1284,7 +1285,7 @@
       <c r="E10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="7" t="n">
@@ -1296,9 +1297,9 @@
       <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B10, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+      <c r="J10" s="7" t="str">
+        <f aca="false" t="array" ref="J10:J10">_xlfn.SWITCH(B10, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>50</v>
@@ -1361,8 +1362,8 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B11, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000110</v>
+        <f aca="false" t="array" ref="J11:J11">_xlfn.SWITCH(B11, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000110</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>25</v>
@@ -1412,7 +1413,7 @@
       <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="n">
@@ -1424,9 +1425,9 @@
       <c r="I12" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B12, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000101</v>
+      <c r="J12" s="7" t="str">
+        <f aca="false" t="array" ref="J12:J12">_xlfn.SWITCH(B12, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000101</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>25</v>
@@ -1489,8 +1490,8 @@
         <v>1</v>
       </c>
       <c r="J13" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B13, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000101</v>
+        <f aca="false" t="array" ref="J13:J13">_xlfn.SWITCH(B13, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000101</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>25</v>
@@ -1540,7 +1541,7 @@
       <c r="E14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="7" t="n">
@@ -1552,9 +1553,9 @@
       <c r="I14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J14" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B14, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000100</v>
+      <c r="J14" s="7" t="str">
+        <f aca="false" t="array" ref="J14:J14">_xlfn.SWITCH(B14, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000100</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>25</v>
@@ -1617,8 +1618,8 @@
         <v>1</v>
       </c>
       <c r="J15" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B15, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000100</v>
+        <f aca="false" t="array" ref="J15:J15">_xlfn.SWITCH(B15, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000100</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>25</v>
@@ -1652,7 +1653,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>61</v>
       </c>
@@ -1668,7 +1669,7 @@
       <c r="E16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="7" t="n">
@@ -1680,9 +1681,9 @@
       <c r="I16" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B16, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00111000</v>
+      <c r="J16" s="7" t="str">
+        <f aca="false" t="array" ref="J16:J16">_xlfn.SWITCH(B16, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>111000</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>25</v>
@@ -1745,8 +1746,8 @@
         <v>1</v>
       </c>
       <c r="J17" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B17, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00111000</v>
+        <f aca="false" t="array" ref="J17:J17">_xlfn.SWITCH(B17, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>111000</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>25</v>
@@ -1796,7 +1797,7 @@
       <c r="E18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="7" t="n">
@@ -1808,9 +1809,9 @@
       <c r="I18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J18" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B18, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000010</v>
+      <c r="J18" s="7" t="str">
+        <f aca="false" t="array" ref="J18:J18">_xlfn.SWITCH(B18, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000010</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>25</v>
@@ -1873,8 +1874,8 @@
         <v>0</v>
       </c>
       <c r="J19" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B19, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000001</v>
+        <f aca="false" t="array" ref="J19:J19">_xlfn.SWITCH(B19, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000001</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>25</v>
@@ -1924,7 +1925,7 @@
       <c r="E20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="7" t="n">
@@ -1936,9 +1937,9 @@
       <c r="I20" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J20" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B20, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00001001</v>
+      <c r="J20" s="7" t="str">
+        <f aca="false" t="array" ref="J20:J20">_xlfn.SWITCH(B20, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>001001</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>25</v>
@@ -2001,8 +2002,8 @@
         <v>1</v>
       </c>
       <c r="J21" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B21, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+        <f aca="false" t="array" ref="J21:J21">_xlfn.SWITCH(B21, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>25</v>
@@ -2013,7 +2014,7 @@
       <c r="M21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="N21" s="10" t="str">
+      <c r="N21" s="11" t="str">
         <f aca="false">IF(C21="R", "01", IF(C21="I", "00", IF(C21="J", "TODO", "")))</f>
         <v>00</v>
       </c>
@@ -2052,7 +2053,7 @@
       <c r="E22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="7" t="n">
+      <c r="F22" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="7" t="n">
@@ -2064,9 +2065,9 @@
       <c r="I22" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J22" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B22, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00011000</v>
+      <c r="J22" s="7" t="str">
+        <f aca="false" t="array" ref="J22:J22">_xlfn.SWITCH(B22, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>25</v>
@@ -2129,8 +2130,8 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B23, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00001000</v>
+        <f aca="false" t="array" ref="J23:J23">_xlfn.SWITCH(B23, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>001000</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>25</v>
@@ -2180,7 +2181,7 @@
       <c r="E24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="7" t="n">
+      <c r="F24" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G24" s="7" t="n">
@@ -2192,9 +2193,9 @@
       <c r="I24" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J24" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B24, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00011000</v>
+      <c r="J24" s="7" t="str">
+        <f aca="false" t="array" ref="J24:J24">_xlfn.SWITCH(B24, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>25</v>
@@ -2257,8 +2258,8 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B25, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00011000</v>
+        <f aca="false" t="array" ref="J25:J25">_xlfn.SWITCH(B25, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>011000</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>25</v>
@@ -2288,7 +2289,7 @@
       <c r="S25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="T25" s="11" t="s">
+      <c r="T25" s="12" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2308,7 +2309,7 @@
       <c r="E26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="7" t="n">
+      <c r="F26" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="7" t="n">
@@ -2320,9 +2321,9 @@
       <c r="I26" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J26" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B26, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+      <c r="J26" s="7" t="str">
+        <f aca="false" t="array" ref="J26:J26">_xlfn.SWITCH(B26, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>25</v>
@@ -2352,7 +2353,7 @@
       <c r="S26" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="T26" s="11" t="s">
+      <c r="T26" s="12" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2385,8 +2386,8 @@
         <v>1</v>
       </c>
       <c r="J27" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B27, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+        <f aca="false" t="array" ref="J27:J27">_xlfn.SWITCH(B27, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>25</v>
@@ -2415,7 +2416,7 @@
       <c r="S27" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="T27" s="11" t="s">
+      <c r="T27" s="12" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2435,7 +2436,7 @@
       <c r="E28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="7" t="n">
+      <c r="F28" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="7" t="n">
@@ -2447,9 +2448,9 @@
       <c r="I28" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J28" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B28, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+      <c r="J28" s="7" t="str">
+        <f aca="false" t="array" ref="J28:J28">_xlfn.SWITCH(B28, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>25</v>
@@ -2479,41 +2480,41 @@
       <c r="S28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T28" s="11" t="s">
+      <c r="T28" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="29" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="10" t="n">
+      <c r="G29" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11" t="n">
         <v>1</v>
       </c>
       <c r="J29" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B29, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+        <f aca="false" t="array" ref="J29:J29">_xlfn.SWITCH(B29, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>86</v>
@@ -2563,7 +2564,7 @@
       <c r="E30" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="7" t="n">
+      <c r="F30" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="7" t="n">
@@ -2575,9 +2576,9 @@
       <c r="I30" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J30" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B30, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+      <c r="J30" s="7" t="str">
+        <f aca="false" t="array" ref="J30:J30">_xlfn.SWITCH(B30, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K30" s="7" t="n">
         <v>10</v>
@@ -2612,19 +2613,19 @@
       </c>
     </row>
     <row r="31" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F31" s="4" t="n">
@@ -2640,8 +2641,8 @@
         <v>1</v>
       </c>
       <c r="J31" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B31, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+        <f aca="false" t="array" ref="J31:J31">_xlfn.SWITCH(B31, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>86</v>
@@ -2691,7 +2692,7 @@
       <c r="E32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="7" t="n">
+      <c r="F32" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="7" t="n">
@@ -2703,9 +2704,9 @@
       <c r="I32" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J32" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B32, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00010000</v>
+      <c r="J32" s="7" t="str">
+        <f aca="false" t="array" ref="J32:J32">_xlfn.SWITCH(B32, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>010000</v>
       </c>
       <c r="K32" s="7" t="n">
         <v>10</v>
@@ -2768,8 +2769,8 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B33, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000010</v>
+        <f aca="false" t="array" ref="J33:J33">_xlfn.SWITCH(B33, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000010</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>25</v>
@@ -2819,7 +2820,7 @@
       <c r="E34" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="7" t="n">
+      <c r="F34" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="7" t="n">
@@ -2831,9 +2832,9 @@
       <c r="I34" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J34" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B34, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00000001</v>
+      <c r="J34" s="7" t="str">
+        <f aca="false" t="array" ref="J34:J34">_xlfn.SWITCH(B34, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "000001", "sra", "001001", "sll", "000010", "and", "000011", "or", "000100", "xor", "000101", "nor", "000110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>000001</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>25</v>
@@ -2896,8 +2897,8 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="str">
-        <f aca="false">_xlfn.SWITCH(B35, "addu", "00000000","add", "00010000", "subu", "00001000","sub", "00011000", "srl", "00000001", "sra", "00001001", "sll", "00000010", "and", "00000011", "or", "00000100", "xor", "00000101", "nor", "00000110", "lui", "00010111",  "slt", "00111000","slti", "00111000","bne","01000000","beq","11000000", "TODO")</f>
-        <v>00001001</v>
+        <f aca="false" t="array" ref="J35:J35">_xlfn.SWITCH(B35, "addu", "000000","add", "010000", "subu", "001000","sub", "011000", "srl", "010001", "sra", "011001", "sll", "010010", "and", "000011", "or", "010100", "xor", "010101", "nor", "010110", "lui", "010111",  "slt", "111000","slti", "111000", "TODO")</f>
+        <v>011001</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>25</v>
@@ -2947,7 +2948,7 @@
       <c r="E36" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="7" t="n">
+      <c r="F36" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G36" s="7" t="n">
@@ -3013,68 +3014,54 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
-      <c r="T37" s="12"/>
+      <c r="T37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="0"/>
-      <c r="G38" s="13" t="s">
+      <c r="H38" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="I38" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="J38" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="K38" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="K38" s="14" t="s">
+      <c r="L38" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="L38" s="14" t="s">
+      <c r="M38" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="M38" s="14" t="s">
+      <c r="N38" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="N38" s="14" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="17"/>
+      <c r="I39" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="O38" s="15" t="s">
+      <c r="J39" s="18" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="0"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="I39" s="16" t="s">
+      <c r="K39" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="L39" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="K39" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="O39" s="18" t="s">
-        <v>110</v>
+      <c r="M39" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="19"/>
+      <c r="J40" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>